<commit_message>
Updated on 01-23-2024 at 18:39
</commit_message>
<xml_diff>
--- a/experiment_3/data/cubic_latex.xlsx
+++ b/experiment_3/data/cubic_latex.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,10 +457,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.918</v>
+        <v>-0.96</v>
       </c>
       <c r="C3" t="n">
-        <v>-3.205</v>
+        <v>-3.587</v>
       </c>
     </row>
     <row r="4">
@@ -468,10 +468,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.837</v>
+        <v>-0.919</v>
       </c>
       <c r="C4" t="n">
-        <v>-2.449</v>
+        <v>-3.156</v>
       </c>
     </row>
     <row r="5">
@@ -479,10 +479,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.755</v>
+        <v>-0.879</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.88</v>
+        <v>-2.858</v>
       </c>
     </row>
     <row r="6">
@@ -490,10 +490,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.673</v>
+        <v>-0.838</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.296</v>
+        <v>-2.492</v>
       </c>
     </row>
     <row r="7">
@@ -501,10 +501,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.592</v>
+        <v>-0.798</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.765</v>
+        <v>-2.131</v>
       </c>
     </row>
     <row r="8">
@@ -512,10 +512,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.51</v>
+        <v>-0.758</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.415</v>
+        <v>-1.905</v>
       </c>
     </row>
     <row r="9">
@@ -523,10 +523,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.429</v>
+        <v>-0.717</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.105</v>
+        <v>-1.676</v>
       </c>
     </row>
     <row r="10">
@@ -534,10 +534,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.347</v>
+        <v>-0.677</v>
       </c>
       <c r="C10" t="n">
-        <v>0.313</v>
+        <v>-1.298</v>
       </c>
     </row>
     <row r="11">
@@ -545,10 +545,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.265</v>
+        <v>-0.636</v>
       </c>
       <c r="C11" t="n">
-        <v>0.476</v>
+        <v>-1.138</v>
       </c>
     </row>
     <row r="12">
@@ -556,10 +556,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.184</v>
+        <v>-0.596</v>
       </c>
       <c r="C12" t="n">
-        <v>3.094</v>
+        <v>1.512</v>
       </c>
     </row>
     <row r="13">
@@ -567,10 +567,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.102</v>
+        <v>-0.556</v>
       </c>
       <c r="C13" t="n">
-        <v>-2.121</v>
+        <v>-3.64</v>
       </c>
     </row>
     <row r="14">
@@ -578,10 +578,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.02</v>
+        <v>-0.515</v>
       </c>
       <c r="C14" t="n">
-        <v>1.057</v>
+        <v>-0.369</v>
       </c>
     </row>
     <row r="15">
@@ -589,10 +589,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.061</v>
+        <v>-0.475</v>
       </c>
       <c r="C15" t="n">
-        <v>0.978</v>
+        <v>-0.33</v>
       </c>
     </row>
     <row r="16">
@@ -600,10 +600,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.143</v>
+        <v>-0.434</v>
       </c>
       <c r="C16" t="n">
-        <v>1.12</v>
+        <v>-0.046</v>
       </c>
     </row>
     <row r="17">
@@ -611,10 +611,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.224</v>
+        <v>-0.394</v>
       </c>
       <c r="C17" t="n">
-        <v>1.182</v>
+        <v>0.177</v>
       </c>
     </row>
     <row r="18">
@@ -622,10 +622,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.306</v>
+        <v>-0.354</v>
       </c>
       <c r="C18" t="n">
-        <v>1.103</v>
+        <v>0.276</v>
       </c>
     </row>
     <row r="19">
@@ -633,10 +633,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.388</v>
+        <v>-0.313</v>
       </c>
       <c r="C19" t="n">
-        <v>0.949</v>
+        <v>0.316</v>
       </c>
     </row>
     <row r="20">
@@ -644,10 +644,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.469</v>
+        <v>-0.273</v>
       </c>
       <c r="C20" t="n">
-        <v>0.96</v>
+        <v>0.532</v>
       </c>
     </row>
     <row r="21">
@@ -655,10 +655,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.551</v>
+        <v>-0.232</v>
       </c>
       <c r="C21" t="n">
-        <v>0.879</v>
+        <v>0.665</v>
       </c>
     </row>
     <row r="22">
@@ -666,10 +666,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.633</v>
+        <v>-0.192</v>
       </c>
       <c r="C22" t="n">
-        <v>0.695</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="23">
@@ -677,10 +677,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.714</v>
+        <v>-0.152</v>
       </c>
       <c r="C23" t="n">
-        <v>0.639</v>
+        <v>0.867</v>
       </c>
     </row>
     <row r="24">
@@ -688,10 +688,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.796</v>
+        <v>-0.111</v>
       </c>
       <c r="C24" t="n">
-        <v>0.361</v>
+        <v>0.8120000000000001</v>
       </c>
     </row>
     <row r="25">
@@ -699,10 +699,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.878</v>
+        <v>-0.07099999999999999</v>
       </c>
       <c r="C25" t="n">
-        <v>0.238</v>
+        <v>0.909</v>
       </c>
     </row>
     <row r="26">
@@ -710,10 +710,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.959</v>
+        <v>-0.03</v>
       </c>
       <c r="C26" t="n">
-        <v>0.028</v>
+        <v>0.913</v>
       </c>
     </row>
     <row r="27">
@@ -721,10 +721,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>1.041</v>
+        <v>0.01</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.12</v>
+        <v>0.971</v>
       </c>
     </row>
     <row r="28">
@@ -732,10 +732,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>1.122</v>
+        <v>0.051</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.201</v>
+        <v>1.085</v>
       </c>
     </row>
     <row r="29">
@@ -743,10 +743,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>1.204</v>
+        <v>0.091</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.401</v>
+        <v>1.066</v>
       </c>
     </row>
     <row r="30">
@@ -754,10 +754,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>1.286</v>
+        <v>0.131</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.599</v>
+        <v>1.031</v>
       </c>
     </row>
     <row r="31">
@@ -765,10 +765,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>1.367</v>
+        <v>0.172</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.7</v>
+        <v>1.073</v>
       </c>
     </row>
     <row r="32">
@@ -776,10 +776,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>1.449</v>
+        <v>0.212</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.795</v>
+        <v>1.099</v>
       </c>
     </row>
     <row r="33">
@@ -787,10 +787,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>1.531</v>
+        <v>0.253</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.895</v>
+        <v>1.094</v>
       </c>
     </row>
     <row r="34">
@@ -798,10 +798,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>1.612</v>
+        <v>0.293</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.983</v>
+        <v>1.073</v>
       </c>
     </row>
     <row r="35">
@@ -809,10 +809,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>1.694</v>
+        <v>0.333</v>
       </c>
       <c r="C35" t="n">
-        <v>-1.088</v>
+        <v>1.002</v>
       </c>
     </row>
     <row r="36">
@@ -820,10 +820,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>1.776</v>
+        <v>0.374</v>
       </c>
       <c r="C36" t="n">
-        <v>-1.058</v>
+        <v>1.034</v>
       </c>
     </row>
     <row r="37">
@@ -831,10 +831,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>1.857</v>
+        <v>0.414</v>
       </c>
       <c r="C37" t="n">
-        <v>-1.037</v>
+        <v>1.018</v>
       </c>
     </row>
     <row r="38">
@@ -842,10 +842,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>1.939</v>
+        <v>0.455</v>
       </c>
       <c r="C38" t="n">
-        <v>-1.072</v>
+        <v>0.907</v>
       </c>
     </row>
     <row r="39">
@@ -853,10 +853,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>2.02</v>
+        <v>0.495</v>
       </c>
       <c r="C39" t="n">
-        <v>-3.997</v>
+        <v>-2.137</v>
       </c>
     </row>
     <row r="40">
@@ -864,10 +864,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>2.102</v>
+        <v>0.535</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.925</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="41">
@@ -875,10 +875,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>2.184</v>
+        <v>0.576</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.705</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="42">
@@ -886,10 +886,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>2.265</v>
+        <v>0.616</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.549</v>
+        <v>0.667</v>
       </c>
     </row>
     <row r="43">
@@ -897,10 +897,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>2.347</v>
+        <v>0.657</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.3</v>
+        <v>0.596</v>
       </c>
     </row>
     <row r="44">
@@ -908,10 +908,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>2.429</v>
+        <v>0.697</v>
       </c>
       <c r="C44" t="n">
-        <v>0.103</v>
+        <v>0.623</v>
       </c>
     </row>
     <row r="45">
@@ -919,10 +919,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>2.51</v>
+        <v>0.737</v>
       </c>
       <c r="C45" t="n">
-        <v>-3.433</v>
+        <v>-3.35</v>
       </c>
     </row>
     <row r="46">
@@ -930,10 +930,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>2.592</v>
+        <v>0.778</v>
       </c>
       <c r="C46" t="n">
-        <v>0.949</v>
+        <v>0.533</v>
       </c>
     </row>
     <row r="47">
@@ -941,10 +941,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>2.673</v>
+        <v>0.8179999999999999</v>
       </c>
       <c r="C47" t="n">
-        <v>1.325</v>
+        <v>0.343</v>
       </c>
     </row>
     <row r="48">
@@ -952,10 +952,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>2.755</v>
+        <v>0.859</v>
       </c>
       <c r="C48" t="n">
-        <v>1.84</v>
+        <v>0.223</v>
       </c>
     </row>
     <row r="49">
@@ -963,10 +963,10 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>2.837</v>
+        <v>0.899</v>
       </c>
       <c r="C49" t="n">
-        <v>2.548</v>
+        <v>0.226</v>
       </c>
     </row>
     <row r="50">
@@ -974,10 +974,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>2.918</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="C50" t="n">
-        <v>3.303</v>
+        <v>0.201</v>
       </c>
     </row>
     <row r="51">
@@ -985,10 +985,560 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.042</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="C52" t="n">
+        <v>-0.029</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>1.061</v>
+      </c>
+      <c r="C53" t="n">
+        <v>-0.091</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>1.101</v>
+      </c>
+      <c r="C54" t="n">
+        <v>-0.169</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1.141</v>
+      </c>
+      <c r="C55" t="n">
+        <v>-0.355</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1.182</v>
+      </c>
+      <c r="C56" t="n">
+        <v>-0.371</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>1.222</v>
+      </c>
+      <c r="C57" t="n">
+        <v>-3.445</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>1.263</v>
+      </c>
+      <c r="C58" t="n">
+        <v>-0.534</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>1.303</v>
+      </c>
+      <c r="C59" t="n">
+        <v>-0.63</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>1.343</v>
+      </c>
+      <c r="C60" t="n">
+        <v>-0.699</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>1.384</v>
+      </c>
+      <c r="C61" t="n">
+        <v>-0.6850000000000001</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>1.424</v>
+      </c>
+      <c r="C62" t="n">
+        <v>-0.695</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>1.465</v>
+      </c>
+      <c r="C63" t="n">
+        <v>-0.896</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>1.505</v>
+      </c>
+      <c r="C64" t="n">
+        <v>-0.856</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>1.545</v>
+      </c>
+      <c r="C65" t="n">
+        <v>-0.872</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>1.586</v>
+      </c>
+      <c r="C66" t="n">
+        <v>-3.737</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>1.626</v>
+      </c>
+      <c r="C67" t="n">
+        <v>-1.067</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>1.667</v>
+      </c>
+      <c r="C68" t="n">
+        <v>-0.954</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>1.707</v>
+      </c>
+      <c r="C69" t="n">
+        <v>-1.09</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>1.747</v>
+      </c>
+      <c r="C70" t="n">
+        <v>-1.016</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>1.788</v>
+      </c>
+      <c r="C71" t="n">
+        <v>-1.055</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>1.828</v>
+      </c>
+      <c r="C72" t="n">
+        <v>-1.067</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="n">
+        <v>1.869</v>
+      </c>
+      <c r="C73" t="n">
+        <v>-1.161</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="n">
+        <v>1.909</v>
+      </c>
+      <c r="C74" t="n">
+        <v>-1.107</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="n">
+        <v>1.949</v>
+      </c>
+      <c r="C75" t="n">
+        <v>-0.971</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="C76" t="n">
+        <v>-4.672</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="C77" t="n">
+        <v>-0.871</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="n">
+        <v>2.071</v>
+      </c>
+      <c r="C78" t="n">
+        <v>-0.983</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="n">
+        <v>2.111</v>
+      </c>
+      <c r="C79" t="n">
+        <v>-0.912</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="n">
+        <v>2.152</v>
+      </c>
+      <c r="C80" t="n">
+        <v>-0.705</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="n">
+        <v>2.192</v>
+      </c>
+      <c r="C81" t="n">
+        <v>-0.723</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="n">
+        <v>2.232</v>
+      </c>
+      <c r="C82" t="n">
+        <v>-3.167</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="n">
+        <v>2.273</v>
+      </c>
+      <c r="C83" t="n">
+        <v>-0.522</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="n">
+        <v>2.313</v>
+      </c>
+      <c r="C84" t="n">
+        <v>-0.305</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="n">
+        <v>2.354</v>
+      </c>
+      <c r="C85" t="n">
+        <v>-0.209</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="n">
+        <v>2.394</v>
+      </c>
+      <c r="C86" t="n">
+        <v>-0.127</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="n">
+        <v>2.434</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0.063</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="n">
+        <v>2.475</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0.211</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="n">
+        <v>2.515</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0.483</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="n">
+        <v>2.556</v>
+      </c>
+      <c r="C90" t="n">
+        <v>-2.431</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="n">
+        <v>2.596</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0.916</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="n">
+        <v>2.636</v>
+      </c>
+      <c r="C92" t="n">
+        <v>1.164</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="n">
+        <v>2.677</v>
+      </c>
+      <c r="C93" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="n">
+        <v>2.717</v>
+      </c>
+      <c r="C94" t="n">
+        <v>3.765</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="n">
+        <v>2.758</v>
+      </c>
+      <c r="C95" t="n">
+        <v>1.857</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="n">
+        <v>2.798</v>
+      </c>
+      <c r="C96" t="n">
+        <v>2.209</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="n">
+        <v>2.838</v>
+      </c>
+      <c r="C97" t="n">
+        <v>-0.491</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="n">
+        <v>2.879</v>
+      </c>
+      <c r="C98" t="n">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="n">
+        <v>2.919</v>
+      </c>
+      <c r="C99" t="n">
+        <v>3.198</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="C100" t="n">
+        <v>3.678</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="n">
         <v>3</v>
       </c>
-      <c r="C51" t="n">
-        <v>4.001</v>
+      <c r="C101" t="n">
+        <v>4.048</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 01-23-2024 at 23:31
</commit_message>
<xml_diff>
--- a/experiment_3/data/cubic_latex.xlsx
+++ b/experiment_3/data/cubic_latex.xlsx
@@ -559,7 +559,7 @@
         <v>-0.596</v>
       </c>
       <c r="C12" t="n">
-        <v>1.512</v>
+        <v>0.158</v>
       </c>
     </row>
     <row r="13">
@@ -570,7 +570,7 @@
         <v>-0.556</v>
       </c>
       <c r="C13" t="n">
-        <v>-3.64</v>
+        <v>-2.045</v>
       </c>
     </row>
     <row r="14">
@@ -856,7 +856,7 @@
         <v>0.495</v>
       </c>
       <c r="C39" t="n">
-        <v>-2.137</v>
+        <v>-0.53</v>
       </c>
     </row>
     <row r="40">
@@ -922,7 +922,7 @@
         <v>0.737</v>
       </c>
       <c r="C45" t="n">
-        <v>-3.35</v>
+        <v>-1.407</v>
       </c>
     </row>
     <row r="46">
@@ -1054,7 +1054,7 @@
         <v>1.222</v>
       </c>
       <c r="C57" t="n">
-        <v>-3.445</v>
+        <v>-1.84</v>
       </c>
     </row>
     <row r="58">
@@ -1153,7 +1153,7 @@
         <v>1.586</v>
       </c>
       <c r="C66" t="n">
-        <v>-3.737</v>
+        <v>-2.23</v>
       </c>
     </row>
     <row r="67">
@@ -1263,7 +1263,7 @@
         <v>1.99</v>
       </c>
       <c r="C76" t="n">
-        <v>-4.672</v>
+        <v>-2.807</v>
       </c>
     </row>
     <row r="77">
@@ -1329,7 +1329,7 @@
         <v>2.232</v>
       </c>
       <c r="C82" t="n">
-        <v>-3.167</v>
+        <v>-1.738</v>
       </c>
     </row>
     <row r="83">
@@ -1417,7 +1417,7 @@
         <v>2.556</v>
       </c>
       <c r="C90" t="n">
-        <v>-2.431</v>
+        <v>-0.797</v>
       </c>
     </row>
     <row r="91">
@@ -1461,7 +1461,7 @@
         <v>2.717</v>
       </c>
       <c r="C94" t="n">
-        <v>3.765</v>
+        <v>2.511</v>
       </c>
     </row>
     <row r="95">
@@ -1494,7 +1494,7 @@
         <v>2.838</v>
       </c>
       <c r="C97" t="n">
-        <v>-0.491</v>
+        <v>1.12</v>
       </c>
     </row>
     <row r="98">

</xml_diff>

<commit_message>
Updated on 01-26-2024 at 07:38
</commit_message>
<xml_diff>
--- a/experiment_3/data/cubic_latex.xlsx
+++ b/experiment_3/data/cubic_latex.xlsx
@@ -559,7 +559,7 @@
         <v>-0.596</v>
       </c>
       <c r="C12" t="n">
-        <v>0.158</v>
+        <v>1.512</v>
       </c>
     </row>
     <row r="13">
@@ -570,7 +570,7 @@
         <v>-0.556</v>
       </c>
       <c r="C13" t="n">
-        <v>-2.045</v>
+        <v>-3.64</v>
       </c>
     </row>
     <row r="14">
@@ -856,7 +856,7 @@
         <v>0.495</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.53</v>
+        <v>-2.137</v>
       </c>
     </row>
     <row r="40">
@@ -922,7 +922,7 @@
         <v>0.737</v>
       </c>
       <c r="C45" t="n">
-        <v>-1.407</v>
+        <v>-3.35</v>
       </c>
     </row>
     <row r="46">
@@ -1054,7 +1054,7 @@
         <v>1.222</v>
       </c>
       <c r="C57" t="n">
-        <v>-1.84</v>
+        <v>-3.445</v>
       </c>
     </row>
     <row r="58">
@@ -1153,7 +1153,7 @@
         <v>1.586</v>
       </c>
       <c r="C66" t="n">
-        <v>-2.23</v>
+        <v>-3.737</v>
       </c>
     </row>
     <row r="67">
@@ -1263,7 +1263,7 @@
         <v>1.99</v>
       </c>
       <c r="C76" t="n">
-        <v>-2.807</v>
+        <v>-4.672</v>
       </c>
     </row>
     <row r="77">
@@ -1329,7 +1329,7 @@
         <v>2.232</v>
       </c>
       <c r="C82" t="n">
-        <v>-1.738</v>
+        <v>-3.167</v>
       </c>
     </row>
     <row r="83">
@@ -1417,7 +1417,7 @@
         <v>2.556</v>
       </c>
       <c r="C90" t="n">
-        <v>-0.797</v>
+        <v>-2.431</v>
       </c>
     </row>
     <row r="91">
@@ -1461,7 +1461,7 @@
         <v>2.717</v>
       </c>
       <c r="C94" t="n">
-        <v>2.511</v>
+        <v>3.765</v>
       </c>
     </row>
     <row r="95">
@@ -1494,7 +1494,7 @@
         <v>2.838</v>
       </c>
       <c r="C97" t="n">
-        <v>1.12</v>
+        <v>-0.491</v>
       </c>
     </row>
     <row r="98">

</xml_diff>

<commit_message>
Updated on 02-02-2024 at 21:47
</commit_message>
<xml_diff>
--- a/experiment_3/data/cubic_latex.xlsx
+++ b/experiment_3/data/cubic_latex.xlsx
@@ -559,7 +559,7 @@
         <v>-0.596</v>
       </c>
       <c r="C12" t="n">
-        <v>1.512</v>
+        <v>0.158</v>
       </c>
     </row>
     <row r="13">
@@ -570,7 +570,7 @@
         <v>-0.556</v>
       </c>
       <c r="C13" t="n">
-        <v>-3.64</v>
+        <v>-2.045</v>
       </c>
     </row>
     <row r="14">
@@ -856,7 +856,7 @@
         <v>0.495</v>
       </c>
       <c r="C39" t="n">
-        <v>-2.137</v>
+        <v>-0.53</v>
       </c>
     </row>
     <row r="40">
@@ -922,7 +922,7 @@
         <v>0.737</v>
       </c>
       <c r="C45" t="n">
-        <v>-3.35</v>
+        <v>-1.407</v>
       </c>
     </row>
     <row r="46">
@@ -1054,7 +1054,7 @@
         <v>1.222</v>
       </c>
       <c r="C57" t="n">
-        <v>-3.445</v>
+        <v>-1.84</v>
       </c>
     </row>
     <row r="58">
@@ -1153,7 +1153,7 @@
         <v>1.586</v>
       </c>
       <c r="C66" t="n">
-        <v>-3.737</v>
+        <v>-2.23</v>
       </c>
     </row>
     <row r="67">
@@ -1263,7 +1263,7 @@
         <v>1.99</v>
       </c>
       <c r="C76" t="n">
-        <v>-4.672</v>
+        <v>-2.807</v>
       </c>
     </row>
     <row r="77">
@@ -1329,7 +1329,7 @@
         <v>2.232</v>
       </c>
       <c r="C82" t="n">
-        <v>-3.167</v>
+        <v>-1.738</v>
       </c>
     </row>
     <row r="83">
@@ -1417,7 +1417,7 @@
         <v>2.556</v>
       </c>
       <c r="C90" t="n">
-        <v>-2.431</v>
+        <v>-0.797</v>
       </c>
     </row>
     <row r="91">
@@ -1461,7 +1461,7 @@
         <v>2.717</v>
       </c>
       <c r="C94" t="n">
-        <v>3.765</v>
+        <v>2.511</v>
       </c>
     </row>
     <row r="95">
@@ -1494,7 +1494,7 @@
         <v>2.838</v>
       </c>
       <c r="C97" t="n">
-        <v>-0.491</v>
+        <v>1.12</v>
       </c>
     </row>
     <row r="98">

</xml_diff>